<commit_message>
Datasource para la validacion de la cola de mensajes. Cambios por la nueva versión de Ranorex
</commit_message>
<xml_diff>
--- a/SuraClaims/AprobacionesPagos.xlsx
+++ b/SuraClaims/AprobacionesPagos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE7FF13-D4BD-4F45-AC30-790A3F12C5A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675B95E7-A887-4903-8426-C52FB3FE23EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D25DB973-7044-4683-AF33-2EEB0F8C9B88}"/>
   </bookViews>
@@ -39,22 +39,22 @@
     <t>Contrasenia</t>
   </si>
   <si>
-    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
-  </si>
-  <si>
-    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
-  </si>
-  <si>
     <t>silverarrow</t>
   </si>
   <si>
     <t>NroSiniestro</t>
   </si>
   <si>
-    <t>rsuarez</t>
-  </si>
-  <si>
-    <t>1220194200610</t>
+    <t>1120170200908</t>
+  </si>
+  <si>
+    <t>dgariffo</t>
+  </si>
+  <si>
+    <t>https://preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
+  </si>
+  <si>
+    <t>preproducciongestion.segurossura.com.ar</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,27 +451,30 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{8A5C6E3D-92C7-40AF-BA0A-2036118EC929}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
validacion generación siniestro SISE
</commit_message>
<xml_diff>
--- a/SuraClaims/AprobacionesPagos.xlsx
+++ b/SuraClaims/AprobacionesPagos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675B95E7-A887-4903-8426-C52FB3FE23EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B1F4A5-62C1-4623-82E5-7DEE3376BFA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D25DB973-7044-4683-AF33-2EEB0F8C9B88}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Ambiente</t>
   </si>
@@ -45,9 +45,6 @@
     <t>NroSiniestro</t>
   </si>
   <si>
-    <t>1120170200908</t>
-  </si>
-  <si>
     <t>dgariffo</t>
   </si>
   <si>
@@ -55,6 +52,18 @@
   </si>
   <si>
     <t>preproducciongestion.segurossura.com.ar</t>
+  </si>
+  <si>
+    <t>1120194100378</t>
+  </si>
+  <si>
+    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
+  </si>
+  <si>
+    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
+  </si>
+  <si>
+    <t>1120194100385</t>
   </si>
 </sst>
 </file>
@@ -426,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9B9E65-C06E-45A4-A7F6-A46B8429DFA4}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,24 +465,41 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{8A5C6E3D-92C7-40AF-BA0A-2036118EC929}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{F7A87B64-591C-4A45-98F8-58ADB0E70F50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
generar litigio (mediación o juicio)
</commit_message>
<xml_diff>
--- a/SuraClaims/AprobacionesPagos.xlsx
+++ b/SuraClaims/AprobacionesPagos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B1F4A5-62C1-4623-82E5-7DEE3376BFA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF05E49-EC22-4916-8E40-17EFCE1FA4C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D25DB973-7044-4683-AF33-2EEB0F8C9B88}"/>
   </bookViews>
@@ -48,22 +48,22 @@
     <t>dgariffo</t>
   </si>
   <si>
+    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
+  </si>
+  <si>
+    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
+  </si>
+  <si>
+    <t>1120194100385</t>
+  </si>
+  <si>
+    <t>preproducciongestion.segurossura.com.ar</t>
+  </si>
+  <si>
     <t>https://preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
   </si>
   <si>
-    <t>preproducciongestion.segurossura.com.ar</t>
-  </si>
-  <si>
-    <t>1120194100378</t>
-  </si>
-  <si>
-    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
-  </si>
-  <si>
-    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
-  </si>
-  <si>
-    <t>1120194100385</t>
+    <t xml:space="preserve">1120170200917  </t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,10 +465,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -477,15 +477,15 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -494,7 +494,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validacion de litigios en SISE
</commit_message>
<xml_diff>
--- a/SuraClaims/AprobacionesPagos.xlsx
+++ b/SuraClaims/AprobacionesPagos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF05E49-EC22-4916-8E40-17EFCE1FA4C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFF9829-F096-4DE5-A8C1-5DC6BB6F2DC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D25DB973-7044-4683-AF33-2EEB0F8C9B88}"/>
   </bookViews>
@@ -63,7 +63,7 @@
     <t>https://preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
   </si>
   <si>
-    <t xml:space="preserve">1120170200917  </t>
+    <t xml:space="preserve">1120170200926  </t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cambios para poder hacer el push
</commit_message>
<xml_diff>
--- a/SuraClaims/AprobacionesPagos.xlsx
+++ b/SuraClaims/AprobacionesPagos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFF9829-F096-4DE5-A8C1-5DC6BB6F2DC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FC32B6-4BEB-4A80-855B-EFFE32CC3BBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D25DB973-7044-4683-AF33-2EEB0F8C9B88}"/>
   </bookViews>
@@ -54,16 +54,16 @@
     <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
   </si>
   <si>
-    <t>1120194100385</t>
-  </si>
-  <si>
     <t>preproducciongestion.segurossura.com.ar</t>
   </si>
   <si>
     <t>https://preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
   </si>
   <si>
-    <t xml:space="preserve">1120170200926  </t>
+    <t>1120194100404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1120170200928  </t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,15 +477,15 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>